<commit_message>
add script to create invoices from excel file
</commit_message>
<xml_diff>
--- a/sendinvoicesinexcelsheet/example.xlsx
+++ b/sendinvoicesinexcelsheet/example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F63306B-DB9B-774E-9B19-8BB7A5C916C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E174AC7-C3CC-AD4C-A8B0-9608548B5093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <t>Invoice Number</t>
   </si>
   <si>
-    <t>DEL-0200056712</t>
+    <t>INV-00010</t>
   </si>
 </sst>
 </file>
@@ -335,10 +335,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>